<commit_message>
Added nupkg for UiPath processes. Integrated RPA process with crewAI agent
</commit_message>
<xml_diff>
--- a/output/vendor_abc_solutions_contract/vendor_abc_solutions_contract_extracted_contract_details.xlsx
+++ b/output/vendor_abc_solutions_contract/vendor_abc_solutions_contract_extracted_contract_details.xlsx
@@ -435,7 +435,7 @@
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="31" customWidth="1" min="2" max="2"/>
-    <col width="149" customWidth="1" min="3" max="3"/>
+    <col width="195" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -638,7 +638,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>Jane Doe, Procurement Manager</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ryan Smith</t>
+          <t>Ryan Smith, CTO</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Not specified</t>
+          <t>Not Specified</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Automatically renew for successive one-year periods unless either party provides written notice of non-renewal at least 15 days prior to expiration</t>
+          <t>This Agreement shall automatically renew for successive one-year periods unless either party provides written notice of non-renewal at least 15 days prior to the expiration of the current term.</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Not specified</t>
+          <t>Not Specified</t>
         </is>
       </c>
     </row>

</xml_diff>